<commit_message>
GBDS OCTOBER 2025 FILES | UPDATED FILES
</commit_message>
<xml_diff>
--- a/GBDS OCTOBER FILES 2025/PURCHASES - OCTOBER.xlsx
+++ b/GBDS OCTOBER FILES 2025/PURCHASES - OCTOBER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GBDS OCTOBER FILES 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12513691-A937-4397-9857-74A304ADBB73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDF2BD2-4DBC-4434-B6D6-129A6DB55B02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2214,7 +2214,7 @@
   <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2519,7 +2519,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C11" s="19"/>
+      <c r="C11" s="19">
+        <v>45945</v>
+      </c>
       <c r="D11" s="20" t="s">
         <v>68</v>
       </c>
@@ -2527,22 +2529,27 @@
       <c r="F11" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="20"/>
+      <c r="G11" s="20">
+        <v>518000493</v>
+      </c>
       <c r="H11" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="I11" s="21"/>
+      <c r="I11" s="21">
+        <f>1327212-56255.04</f>
+        <v>1270956.96</v>
+      </c>
       <c r="K11" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>136173.96</v>
       </c>
       <c r="L11" s="27">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1134783</v>
       </c>
       <c r="M11" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11347.83</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -3133,19 +3140,19 @@
       <c r="G32"/>
       <c r="I32" s="14">
         <f>SUM(I7:I31)</f>
-        <v>5160925.26</v>
+        <v>6431882.2199999997</v>
       </c>
       <c r="K32" s="14">
         <f>SUM(K7:K31)</f>
-        <v>552956.27785714285</v>
+        <v>689130.23785714281</v>
       </c>
       <c r="L32" s="14">
         <f>SUM(L7:L31)</f>
-        <v>4607968.9821428573</v>
+        <v>5742751.9821428573</v>
       </c>
       <c r="M32" s="36">
         <f>SUM(M7:M31)</f>
-        <v>46079.689821428561</v>
+        <v>57427.519821428563</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>